<commit_message>
Corrected error in execution time calculation
</commit_message>
<xml_diff>
--- a/Project 2/Miss_Rates_and_Exec_Time.xlsx
+++ b/Project 2/Miss_Rates_and_Exec_Time.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Long Trace 1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -208,7 +208,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -217,23 +228,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -301,7 +301,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -448,11 +447,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1142312464"/>
-        <c:axId val="-1148787872"/>
+        <c:axId val="-125962336"/>
+        <c:axId val="-129335232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1142312464"/>
+        <c:axId val="-125962336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +494,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1148787872"/>
+        <c:crossAx val="-129335232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -503,7 +502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1148787872"/>
+        <c:axId val="-129335232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +552,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1142312464"/>
+        <c:crossAx val="-125962336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -567,7 +566,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -679,7 +677,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -826,11 +823,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1142358208"/>
-        <c:axId val="-1121045040"/>
+        <c:axId val="-126000064"/>
+        <c:axId val="-125975360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1142358208"/>
+        <c:axId val="-126000064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1121045040"/>
+        <c:crossAx val="-125975360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -881,7 +878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1121045040"/>
+        <c:axId val="-125975360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1142358208"/>
+        <c:crossAx val="-126000064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -945,7 +942,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2428,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2438,359 +2434,311 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="5">
         <f>B11*100</f>
         <v>0.46299999999999997</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="5">
         <f t="shared" ref="C3:J3" si="0">C11*100</f>
         <v>1.7700000000000001E-3</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="5">
         <f t="shared" si="0"/>
         <v>1.8E-3</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="5">
         <f t="shared" si="0"/>
         <v>25.900000000000002</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="5">
         <f t="shared" si="0"/>
         <v>18.221</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" si="0"/>
-        <v>38861893900</v>
-      </c>
-      <c r="I3" s="9">
-        <f t="shared" si="0"/>
-        <v>31069585900</v>
-      </c>
-      <c r="J3" s="9">
-        <f t="shared" si="0"/>
-        <v>25891823900</v>
+      <c r="H3" s="4">
+        <f>388618939</f>
+        <v>388618939</v>
+      </c>
+      <c r="I3" s="4">
+        <v>310695859</v>
+      </c>
+      <c r="J3" s="4">
+        <v>258918239</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <f t="shared" ref="B4:J6" si="1">B12*100</f>
         <v>1.6957</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <f t="shared" si="1"/>
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <f t="shared" si="1"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>31.1525</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <f t="shared" si="1"/>
         <v>18.096599999999999</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="5">
         <f t="shared" si="1"/>
         <v>10.647500000000001</v>
       </c>
-      <c r="H4" s="9">
-        <f t="shared" si="1"/>
-        <v>36937987900</v>
-      </c>
-      <c r="I4" s="9">
-        <f t="shared" si="1"/>
-        <v>24312345900</v>
-      </c>
-      <c r="J4" s="9">
-        <f t="shared" si="1"/>
-        <v>19311783900</v>
-      </c>
-      <c r="L4" s="13" t="s">
+      <c r="H4" s="4">
+        <v>369379879</v>
+      </c>
+      <c r="I4" s="4">
+        <v>243123459</v>
+      </c>
+      <c r="J4" s="4">
+        <v>193117839</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="5">
         <f t="shared" si="1"/>
         <v>3.0387999999999997</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="5">
         <f t="shared" si="1"/>
         <v>1.9999999999999998E-4</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="5">
         <f t="shared" si="1"/>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>48.555199999999999</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <f t="shared" si="1"/>
         <v>16.108000000000001</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>8.301400000000001</v>
       </c>
-      <c r="H5" s="9">
-        <f t="shared" si="1"/>
-        <v>53613195900</v>
-      </c>
-      <c r="I5" s="9">
-        <f t="shared" si="1"/>
-        <v>22627049900</v>
-      </c>
-      <c r="J5" s="9">
-        <f t="shared" si="1"/>
-        <v>17334305900</v>
+      <c r="H5" s="4">
+        <v>536131959</v>
+      </c>
+      <c r="I5" s="4">
+        <v>226270499</v>
+      </c>
+      <c r="J5" s="4">
+        <v>173343059</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="5">
         <f t="shared" si="1"/>
         <v>3.3050999999999995</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <f t="shared" si="1"/>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <f t="shared" si="1"/>
         <v>67.162300000000002</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <f t="shared" si="1"/>
         <v>17.006</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>7.7254000000000005</v>
       </c>
-      <c r="H6" s="9">
-        <f t="shared" si="1"/>
-        <v>70394625900</v>
-      </c>
-      <c r="I6" s="9">
-        <f t="shared" si="1"/>
-        <v>23332567900</v>
-      </c>
-      <c r="J6" s="9">
-        <f t="shared" si="1"/>
-        <v>16848905900</v>
+      <c r="H6" s="4">
+        <v>703946259</v>
+      </c>
+      <c r="I6" s="4">
+        <v>233325679</v>
+      </c>
+      <c r="J6" s="4">
+        <v>168489059</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="9">
+      <c r="B11" s="5">
         <v>4.6299999999999996E-3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="5">
         <v>1.77E-5</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="5">
         <v>1.8E-5</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>0.36</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="5">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="5">
         <v>0.18221000000000001</v>
-      </c>
-      <c r="H11" s="8">
-        <f>388618939</f>
-        <v>388618939</v>
-      </c>
-      <c r="I11" s="8">
-        <v>310695859</v>
-      </c>
-      <c r="J11" s="8">
-        <v>258918239</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
+      <c r="B12" s="5">
         <v>1.6957E-2</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>0.311525</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="5">
         <v>0.18096599999999999</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="5">
         <v>0.106475</v>
-      </c>
-      <c r="H12" s="8">
-        <v>369379879</v>
-      </c>
-      <c r="I12" s="8">
-        <v>243123459</v>
-      </c>
-      <c r="J12" s="8">
-        <v>193117839</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="9">
+      <c r="B13" s="5">
         <v>3.0387999999999998E-2</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="5">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>0.48555199999999998</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="5">
         <v>0.16108</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="5">
         <v>8.3014000000000004E-2</v>
-      </c>
-      <c r="H13" s="8">
-        <v>536131959</v>
-      </c>
-      <c r="I13" s="8">
-        <v>226270499</v>
-      </c>
-      <c r="J13" s="8">
-        <v>173343059</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="9">
+      <c r="B14" s="5">
         <v>3.3050999999999997E-2</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>0</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>0.67162299999999997</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="5">
         <v>0.17005999999999999</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <v>7.7254000000000003E-2</v>
-      </c>
-      <c r="H14" s="8">
-        <v>703946259</v>
-      </c>
-      <c r="I14" s="8">
-        <v>233325679</v>
-      </c>
-      <c r="J14" s="8">
-        <v>168489059</v>
       </c>
     </row>
   </sheetData>
@@ -2799,7 +2747,7 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2810,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2821,348 +2769,300 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="5">
         <f>B11*100</f>
         <v>0.69141740000000007</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="5">
         <f>C11*100</f>
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="5">
         <f>D11*100</f>
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="5">
         <f t="shared" ref="E3:J3" si="0">E11*100</f>
         <v>60.910470100000005</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="5">
         <f t="shared" si="0"/>
         <v>53.432400000000001</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="5">
         <f t="shared" si="0"/>
         <v>46.560600000000001</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" si="0"/>
-        <v>69847447600</v>
+        <v>698474476</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" si="0"/>
-        <v>61756419600</v>
+        <v>617564196</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" si="0"/>
-        <v>55690603600</v>
-      </c>
-      <c r="M3" s="13"/>
+        <v>556906036</v>
+      </c>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <f t="shared" ref="B4:C4" si="1">B12*100</f>
         <v>0.1953</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <f t="shared" si="1"/>
         <v>1.9999999999999998E-4</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <f t="shared" ref="D4:F4" si="2">D12*100</f>
         <v>1.9999999999999998E-4</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <f t="shared" si="2"/>
         <v>58.1492</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <f t="shared" si="2"/>
         <v>53.767499999999998</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="5">
         <f t="shared" ref="G4:J4" si="3">G12*100</f>
         <v>47.191200000000002</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="3"/>
-        <v>65647481600</v>
+        <v>656474816</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="3"/>
-        <v>61678609600</v>
+        <v>616786096</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="3"/>
-        <v>56055601600</v>
-      </c>
-      <c r="L4" s="13" t="s">
+        <v>560556016</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="5">
         <f t="shared" ref="B5:C5" si="4">B13*100</f>
         <v>5.7499999999999996E-2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="5">
         <f t="shared" ref="D5:F5" si="5">D13*100</f>
         <v>0</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <f t="shared" si="5"/>
         <v>53.850299999999997</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <f t="shared" si="5"/>
         <v>44.982100000000003</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="5">
         <f t="shared" ref="G5:J5" si="6">G13*100</f>
         <v>41.868699999999997</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="6"/>
-        <v>61686609600</v>
+        <v>616866096</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="6"/>
-        <v>54479033600</v>
+        <v>544790336</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="6"/>
-        <v>51743975600</v>
+        <v>517439756</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="5">
         <f t="shared" ref="B6:C6" si="7">B14*100</f>
         <v>2.12E-2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <f t="shared" ref="D6:F6" si="8">D14*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <f t="shared" si="8"/>
         <v>52.047900000000006</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <f t="shared" si="8"/>
         <v>24.2393</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="5">
         <f t="shared" ref="G6:J6" si="9">G14*100</f>
         <v>21.8507</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="9"/>
-        <v>56009753600</v>
+        <v>560097536</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="9"/>
-        <v>33332515600</v>
+        <v>333325156</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="9"/>
-        <v>31188585600</v>
+        <v>311885856</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="9">
+      <c r="B11" s="5">
         <v>6.9141740000000004E-3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="5">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="5">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>0.60910470100000003</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="5">
         <v>0.53432400000000002</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="5">
         <v>0.46560600000000002</v>
-      </c>
-      <c r="H11" s="1">
-        <v>698474476</v>
-      </c>
-      <c r="I11" s="1">
-        <v>617564196</v>
-      </c>
-      <c r="J11" s="1">
-        <v>556906036</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
+      <c r="B12" s="5">
         <v>1.9530000000000001E-3</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>0.58149200000000001</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="5">
         <v>0.53767500000000001</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="5">
         <v>0.471912</v>
-      </c>
-      <c r="H12" s="1">
-        <v>656474816</v>
-      </c>
-      <c r="I12" s="1">
-        <v>616786096</v>
-      </c>
-      <c r="J12" s="1">
-        <v>560556016</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="9">
+      <c r="B13" s="5">
         <v>5.7499999999999999E-4</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="5">
         <v>0</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>0.53850299999999995</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="5">
         <v>0.44982100000000003</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="5">
         <v>0.41868699999999998</v>
-      </c>
-      <c r="H13" s="1">
-        <v>616866096</v>
-      </c>
-      <c r="I13" s="1">
-        <v>544790336</v>
-      </c>
-      <c r="J13" s="1">
-        <v>517439756</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="9">
+      <c r="B14" s="5">
         <v>2.12E-4</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>0</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>0</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>0.52047900000000002</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="5">
         <v>0.242393</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <v>0.21850700000000001</v>
-      </c>
-      <c r="H14" s="1">
-        <v>560097536</v>
-      </c>
-      <c r="I14" s="1">
-        <v>333325156</v>
-      </c>
-      <c r="J14" s="1">
-        <v>311885856</v>
       </c>
     </row>
   </sheetData>
@@ -3171,7 +3071,7 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3192,52 +3092,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>4</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>8</v>
       </c>
     </row>
@@ -3245,15 +3145,15 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="6">
         <f>0.000006*100</f>
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="6">
         <f>0.000003*100</f>
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="6">
         <f>0.000003*100</f>
         <v>3.0000000000000003E-4</v>
       </c>
@@ -3277,14 +3177,14 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="6">
         <f>0.184844*100</f>
         <v>18.484400000000001</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="6">
         <v>14.641400000000001</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="6">
         <v>14.4588</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -3304,15 +3204,15 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="12">
+      <c r="B8" s="7">
         <f>0.000006*100</f>
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="7">
         <f>0.184844*100</f>
         <v>18.484400000000001</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="7"/>
       <c r="G8">
         <v>1E-4</v>
       </c>
@@ -3321,14 +3221,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="12">
+      <c r="B9" s="7">
         <f>0.000003*100</f>
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="7">
         <v>14.641400000000001</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="7"/>
       <c r="G9">
         <v>1E-4</v>
       </c>
@@ -3337,14 +3237,14 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="12">
+      <c r="B10" s="7">
         <f>0.000003*100</f>
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="7">
         <v>14.4588</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="7"/>
       <c r="G10">
         <v>1E-4</v>
       </c>

</xml_diff>